<commit_message>
Added 3D coincident plot
</commit_message>
<xml_diff>
--- a/Tables/MG_to_VMM_Mapping.xlsx
+++ b/Tables/MG_to_VMM_Mapping.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridVMM/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18A25BA3-D0EA-8446-9479-8ED30A75487A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E616D7E9-FF8C-A843-B490-279053973271}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="0" windowWidth="18040" windowHeight="18000" xr2:uid="{EBF7798D-A1F0-5C48-B5D8-45AE0A8C0DD6}"/>
+    <workbookView xWindow="7380" yWindow="820" windowWidth="18040" windowHeight="16360" xr2:uid="{EBF7798D-A1F0-5C48-B5D8-45AE0A8C0DD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>